<commit_message>
updates based on new CSV (9/15 version)
</commit_message>
<xml_diff>
--- a/Downstream_Timeline.xlsx
+++ b/Downstream_Timeline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Rockefeller Philanthropy Advisors</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Not Started</t>
+  </si>
+  <si>
+    <t>At Risk</t>
   </si>
 </sst>
 </file>
@@ -79,7 +82,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,6 +140,17 @@
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF800000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -167,7 +181,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FF800000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,7 +215,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -217,8 +231,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -645,7 +661,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -764,7 +780,7 @@
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="12"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -778,7 +794,7 @@
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="15"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -793,7 +809,7 @@
       <c r="D15" s="10"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="12"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="12"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
@@ -808,7 +824,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="12"/>
+      <c r="H16" s="9"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
     </row>
@@ -822,7 +838,7 @@
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="12"/>
+      <c r="H17" s="9"/>
       <c r="I17" s="12"/>
       <c r="J17" s="10"/>
     </row>
@@ -836,7 +852,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="12"/>
+      <c r="H18" s="9"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
     </row>
@@ -863,8 +879,14 @@
         <v>14</v>
       </c>
     </row>
+    <row r="23" spans="1:15">
+      <c r="F23" s="17"/>
+      <c r="G23" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="31" spans="1:15">
-      <c r="O31" s="16"/>
+      <c r="O31" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updates to support freq table
</commit_message>
<xml_diff>
--- a/Downstream_Timeline.xlsx
+++ b/Downstream_Timeline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Rockefeller Philanthropy Advisors</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>At Risk</t>
+  </si>
+  <si>
+    <t>Postponed</t>
   </si>
 </sst>
 </file>
@@ -154,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +185,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF800000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,7 +224,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -232,9 +241,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -660,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -669,36 +679,36 @@
     <col min="1" max="1" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="133" customHeight="1"/>
-    <row r="2" spans="1:10">
+    <row r="1" spans="1:11" ht="133" customHeight="1"/>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18">
+    <row r="4" spans="1:11" ht="18">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18">
+    <row r="5" spans="1:11" ht="18">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="25">
+    <row r="6" spans="1:11" ht="25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -729,8 +739,11 @@
       <c r="J9" s="8">
         <v>42643</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="8">
+        <v>42650</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="8" t="s">
         <v>4</v>
       </c>
@@ -743,8 +756,9 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="8" t="s">
         <v>5</v>
       </c>
@@ -757,8 +771,9 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="8" t="s">
         <v>6</v>
       </c>
@@ -771,8 +786,9 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
@@ -785,8 +801,9 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
@@ -794,13 +811,14 @@
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="16"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
@@ -810,11 +828,12 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="10"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="10"/>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="8" t="s">
         <v>10</v>
       </c>
@@ -825,8 +844,9 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="10"/>
+      <c r="I16" s="9"/>
       <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="8" t="s">
@@ -840,7 +860,8 @@
       <c r="G17" s="10"/>
       <c r="H17" s="9"/>
       <c r="I17" s="12"/>
-      <c r="J17" s="10"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="8" t="s">
@@ -853,8 +874,9 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="12"/>
+      <c r="I18" s="9"/>
       <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="6"/>
@@ -880,9 +902,15 @@
       </c>
     </row>
     <row r="23" spans="1:15">
-      <c r="F23" s="17"/>
-      <c r="G23" s="18" t="s">
+      <c r="F23" s="16"/>
+      <c r="G23" s="17" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="F24" s="19"/>
+      <c r="G24" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:15">

</xml_diff>